<commit_message>
20170517 list fw rules sorted by position
</commit_message>
<xml_diff>
--- a/conf/fw-rules.xlsx
+++ b/conf/fw-rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>FWaaSルール</t>
   </si>
@@ -130,22 +130,25 @@
     <t>iida-az1-p01-net02-any-tcp</t>
   </si>
   <si>
-    <t>9a7080ae-3c90-4ccc-8659-1b45fbcb7206</t>
+    <t>618c64c3-f28b-404a-ad62-7bec33d7f48b</t>
   </si>
   <si>
     <t>10.1.2.0/24</t>
   </si>
   <si>
+    <t>af2641ee-9637-4e3d-b661-0b4323c138b5</t>
+  </si>
+  <si>
     <t>iida-az1-p01-net02-any-udp</t>
   </si>
   <si>
-    <t>66ffc217-7018-4bef-b1e6-af77e296278d</t>
+    <t>b7077240-adb1-4216-8983-6aa3f1e48d01</t>
   </si>
   <si>
     <t>iida-az1-p01-net02-any-icmp</t>
   </si>
   <si>
-    <t>630cdb7f-16c1-4bbd-83cc-9cd300f42bef</t>
+    <t>9d4138ed-3236-4d50-a637-762b22ffc716</t>
   </si>
   <si>
     <t>中→高</t>
@@ -154,7 +157,7 @@
     <t>iida-az1-p01-net01-net02-tcp</t>
   </si>
   <si>
-    <t>78f5028e-f6f6-4e7b-a6ea-7843805fd6d9</t>
+    <t>0c48089e-f8f2-4eb5-ab4e-f40bf11b91aa</t>
   </si>
   <si>
     <t>deny</t>
@@ -166,13 +169,13 @@
     <t>iida-az1-p01-net01-net02-udp</t>
   </si>
   <si>
-    <t>33b287ac-74f3-4de5-8c28-3aa13d8ee5a5</t>
+    <t>76dcbfc1-6593-4c9a-91b9-ff7223f4d358</t>
   </si>
   <si>
     <t>iida-az1-p01-net01-net02-icmp</t>
   </si>
   <si>
-    <t>7caf076b-5027-407a-9795-90450735ec36</t>
+    <t>d621e8bf-c9c6-485c-b96c-7a09887935fe</t>
   </si>
   <si>
     <t>中→低</t>
@@ -181,19 +184,19 @@
     <t>iida-az1-p01-net01-any-tcp</t>
   </si>
   <si>
-    <t>042c5bff-c7de-4465-9559-b78eb062aa78</t>
+    <t>abded572-ed04-4527-a6b2-1f728a926a81</t>
   </si>
   <si>
     <t>iida-az1-p01-net01-any-udp</t>
   </si>
   <si>
-    <t>76c9313d-e432-4f8b-b5ea-b9e3e36cb767</t>
+    <t>5ef0625e-3f85-435e-a5e7-e1812ffbc173</t>
   </si>
   <si>
     <t>iida-az1-p01-net01-any-icmp</t>
   </si>
   <si>
-    <t>32dae3c1-0d5f-45ab-b8c6-199a1244581a</t>
+    <t>af357dcf-2d4e-4c02-8ec5-3db261665daf</t>
   </si>
   <si>
     <t>明示的deny</t>
@@ -202,19 +205,19 @@
     <t>deny-all-tcp</t>
   </si>
   <si>
-    <t>a5ecfd2b-c62a-45c4-aaa2-dffd0cb7df94</t>
+    <t>cd2249f9-9f7a-42e5-94cb-8a528abeae04</t>
   </si>
   <si>
     <t>deny-all-udp</t>
   </si>
   <si>
-    <t>22472679-548e-482e-ae59-48cc4f210c78</t>
+    <t>5925fef4-392b-4ff6-9962-94a79e8a9973</t>
   </si>
   <si>
     <t>deny-all-icmp</t>
   </si>
   <si>
-    <t>2a391d37-77b5-450d-b04b-76dd3340aad0</t>
+    <t>0b429ceb-e665-48f9-b695-2c0ca9357bea</t>
   </si>
 </sst>
 </file>
@@ -867,15 +870,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ22"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="B1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
       <selection activeCell="D11" activeCellId="0" pane="topLeft" sqref="D11:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="11.0463917525773"/>
+    <col customWidth="1" max="1" min="1" style="3" width="10.7731958762887"/>
     <col customWidth="1" max="2" min="2" style="3" width="9.13917525773196"/>
-    <col customWidth="1" max="3" min="3" style="3" width="31.639175257732"/>
+    <col customWidth="1" max="3" min="3" style="3" width="31.5051546391753"/>
     <col customWidth="1" max="4" min="4" style="3" width="19.0927835051546"/>
     <col customWidth="1" max="5" min="5" style="3" width="9.273195876288661"/>
     <col customWidth="1" max="6" min="6" style="3" width="7.3659793814433"/>
@@ -883,7 +886,7 @@
     <col customWidth="1" max="8" min="8" style="3" width="9.953608247422681"/>
     <col customWidth="1" max="9" min="9" style="3" width="21.4123711340206"/>
     <col customWidth="1" max="10" min="10" style="3" width="13.3659793814433"/>
-    <col customWidth="1" max="11" min="11" style="3" width="13.7731958762887"/>
+    <col customWidth="1" max="11" min="11" style="3" width="13.5"/>
     <col customWidth="1" max="12" min="12" style="3" width="10.3659793814433"/>
     <col customWidth="1" max="15" min="13" style="3" width="13.3659793814433"/>
     <col customWidth="1" max="1025" min="16" style="3" width="7.3659793814433"/>
@@ -1132,7 +1135,9 @@
       <c r="N11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="22" t="n"/>
+      <c r="O11" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="P11" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="12" s="49" spans="1:1024">
@@ -1141,10 +1146,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" s="25" t="n">
         <v>1</v>
@@ -1174,7 +1179,9 @@
       <c r="N12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="27" t="n"/>
+      <c r="O12" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="P12" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="13" s="49" spans="1:1024">
@@ -1183,10 +1190,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="30" t="n">
         <v>1</v>
@@ -1216,27 +1223,29 @@
       <c r="N13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="33" t="n"/>
+      <c r="O13" s="33" t="s">
+        <v>40</v>
+      </c>
       <c r="P13" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="14" s="49" spans="1:1024">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="34" t="n">
         <v>4</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" s="36" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G14" s="38" t="n">
         <v>4</v>
@@ -1245,7 +1254,7 @@
         <v>31</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J14" s="38" t="s">
         <v>32</v>
@@ -1260,7 +1269,9 @@
       <c r="N14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="39" t="n"/>
+      <c r="O14" s="39" t="s">
+        <v>40</v>
+      </c>
       <c r="P14" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="15" s="49" spans="1:1024">
@@ -1269,16 +1280,16 @@
         <v>5</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G15" s="26" t="n">
         <v>4</v>
@@ -1287,7 +1298,7 @@
         <v>34</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J15" s="26" t="s">
         <v>32</v>
@@ -1302,7 +1313,9 @@
       <c r="N15" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O15" s="27" t="n"/>
+      <c r="O15" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="P15" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="16" s="49" spans="1:1024">
@@ -1311,16 +1324,16 @@
         <v>6</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E16" s="43" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G16" s="45" t="n">
         <v>4</v>
@@ -1329,7 +1342,7 @@
         <v>35</v>
       </c>
       <c r="I16" s="45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J16" s="45" t="s">
         <v>32</v>
@@ -1344,21 +1357,23 @@
       <c r="N16" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="46" t="n"/>
+      <c r="O16" s="46" t="s">
+        <v>40</v>
+      </c>
       <c r="P16" s="3" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="17" s="49" spans="1:1024">
       <c r="A17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="34" t="n">
         <v>7</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E17" s="36" t="n">
         <v>1</v>
@@ -1373,7 +1388,7 @@
         <v>31</v>
       </c>
       <c r="I17" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J17" s="38" t="s">
         <v>32</v>
@@ -1388,7 +1403,9 @@
       <c r="N17" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="39" t="n"/>
+      <c r="O17" s="39" t="s">
+        <v>40</v>
+      </c>
       <c r="P17" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="18" s="49" spans="1:1024">
@@ -1397,10 +1414,10 @@
         <v>8</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" s="25" t="n">
         <v>1</v>
@@ -1415,7 +1432,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J18" s="26" t="s">
         <v>32</v>
@@ -1430,7 +1447,9 @@
       <c r="N18" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="27" t="n"/>
+      <c r="O18" s="27" t="s">
+        <v>40</v>
+      </c>
       <c r="P18" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="19" s="49" spans="1:1024">
@@ -1439,10 +1458,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E19" s="43" t="n">
         <v>1</v>
@@ -1457,7 +1476,7 @@
         <v>35</v>
       </c>
       <c r="I19" s="45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J19" s="45" t="s">
         <v>32</v>
@@ -1472,27 +1491,29 @@
       <c r="N19" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="O19" s="46" t="n"/>
+      <c r="O19" s="46" t="s">
+        <v>40</v>
+      </c>
       <c r="P19" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="15.95" r="20" s="49" spans="1:1024">
       <c r="A20" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B20" s="34" t="n">
         <v>10</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" s="36" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="38" t="n">
         <v>4</v>
@@ -1516,23 +1537,25 @@
       <c r="N20" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O20" s="39" t="n"/>
+      <c r="O20" s="39" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" ht="15.95" r="21" s="49" spans="1:1024">
       <c r="B21" s="23" t="n">
         <v>11</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E21" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="40" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G21" s="26" t="n">
         <v>4</v>
@@ -1556,23 +1579,25 @@
       <c r="N21" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="27" t="n"/>
+      <c r="O21" s="27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row customHeight="1" ht="15.95" r="22" s="49" spans="1:1024">
       <c r="B22" s="41" t="n">
         <v>12</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="43" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G22" s="45" t="n">
         <v>4</v>
@@ -1596,7 +1621,9 @@
       <c r="N22" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="O22" s="46" t="n"/>
+      <c r="O22" s="46" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>